<commit_message>
changing temaplates and code for promo displays calculations
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Supermarket PoS 2018.xlsx
+++ b/Projects/CCRU/Data/Supermarket PoS 2018.xlsx
@@ -41,6 +41,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Supermarket!$A$1:$AR$234</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Supermarket!$A$1:$AR$234</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Supermarket!$A$1:$AR$234</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Supermarket!$A$1:$AR$234</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3429" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3430" uniqueCount="668">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -2039,10 +2040,13 @@
     <t xml:space="preserve">Промо дисплеи: Фейсинги</t>
   </si>
   <si>
+    <t xml:space="preserve">check_number_of_scenes_with_facings_target</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COUNT</t>
+  </si>
+  <si>
     <t xml:space="preserve">number of scenes with have at least target amount of facings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COUNT</t>
   </si>
   <si>
     <t xml:space="preserve">Hidden</t>
@@ -3208,21 +3212,21 @@
   <dimension ref="A1:AQ65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AO235" activeCellId="0" sqref="AO235"/>
+      <selection pane="bottomLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.1052631578947"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.2550607287449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.3522267206478"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="13" min="11" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="34" min="16" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="35" min="35" style="0" width="13.8178137651822"/>
     <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="9.10526315789474"/>
@@ -22010,14 +22014,16 @@
       <c r="H219" s="113" t="s">
         <v>607</v>
       </c>
-      <c r="I219" s="118" t="s">
+      <c r="I219" s="81" t="s">
         <v>608</v>
       </c>
       <c r="J219" s="118"/>
       <c r="K219" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="L219" s="58" t="n">
         <v>8</v>
       </c>
-      <c r="L219" s="58"/>
       <c r="M219" s="58"/>
       <c r="N219" s="58" t="s">
         <v>308</v>
@@ -22056,7 +22062,9 @@
       </c>
       <c r="AG219" s="58"/>
       <c r="AH219" s="58"/>
-      <c r="AI219" s="58"/>
+      <c r="AI219" s="57" t="s">
+        <v>610</v>
+      </c>
       <c r="AJ219" s="58"/>
       <c r="AK219" s="58"/>
       <c r="AL219" s="14" t="n">
@@ -22083,23 +22091,23 @@
         <v>44</v>
       </c>
       <c r="D220" s="120" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E220" s="121" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="F220" s="121" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="G220" s="121" t="s">
         <v>402</v>
       </c>
       <c r="H220" s="122"/>
       <c r="I220" s="36" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="J220" s="123" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="K220" s="124"/>
       <c r="L220" s="124"/>
@@ -22110,7 +22118,7 @@
       <c r="Q220" s="124"/>
       <c r="R220" s="124"/>
       <c r="S220" s="124" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="T220" s="124"/>
       <c r="U220" s="124"/>
@@ -22138,7 +22146,7 @@
         <v>219</v>
       </c>
       <c r="AO220" s="123" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="AP220" s="124"/>
       <c r="AQ220" s="124"/>
@@ -22154,23 +22162,23 @@
         <v>44</v>
       </c>
       <c r="D221" s="120" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E221" s="127" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="F221" s="127" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="G221" s="128" t="s">
         <v>321</v>
       </c>
       <c r="H221" s="128"/>
       <c r="I221" s="43" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="J221" s="124" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="K221" s="124"/>
       <c r="L221" s="124"/>
@@ -22181,7 +22189,7 @@
       <c r="Q221" s="124"/>
       <c r="R221" s="124"/>
       <c r="S221" s="124" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="T221" s="124"/>
       <c r="U221" s="124"/>
@@ -22209,7 +22217,7 @@
         <v>220</v>
       </c>
       <c r="AO221" s="123" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="AP221" s="124"/>
       <c r="AQ221" s="124"/>
@@ -22225,25 +22233,25 @@
         <v>44</v>
       </c>
       <c r="D222" s="120" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E222" s="121" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="F222" s="121" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="G222" s="129" t="s">
         <v>589</v>
       </c>
       <c r="H222" s="128" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="I222" s="43" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="J222" s="124" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="K222" s="124"/>
       <c r="L222" s="124"/>
@@ -22254,7 +22262,7 @@
       <c r="Q222" s="124"/>
       <c r="R222" s="124"/>
       <c r="S222" s="124" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="T222" s="124"/>
       <c r="U222" s="124"/>
@@ -22298,23 +22306,23 @@
         <v>44</v>
       </c>
       <c r="D223" s="120" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E223" s="121" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="F223" s="121" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="G223" s="121" t="s">
         <v>539</v>
       </c>
       <c r="H223" s="128"/>
       <c r="I223" s="43" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="J223" s="124" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="K223" s="124"/>
       <c r="L223" s="124"/>
@@ -22325,7 +22333,7 @@
       <c r="Q223" s="124"/>
       <c r="R223" s="124"/>
       <c r="S223" s="124" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="T223" s="124"/>
       <c r="U223" s="124"/>
@@ -22353,7 +22361,7 @@
         <v>222</v>
       </c>
       <c r="AO223" s="123" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="AP223" s="124"/>
       <c r="AQ223" s="124"/>
@@ -22369,25 +22377,25 @@
         <v>44</v>
       </c>
       <c r="D224" s="120" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E224" s="121" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="F224" s="121" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="G224" s="121" t="s">
         <v>605</v>
       </c>
       <c r="H224" s="128" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="I224" s="43" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="J224" s="124" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="K224" s="124"/>
       <c r="L224" s="124"/>
@@ -22398,7 +22406,7 @@
       <c r="Q224" s="124"/>
       <c r="R224" s="124"/>
       <c r="S224" s="124" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="T224" s="124"/>
       <c r="U224" s="124"/>
@@ -22442,36 +22450,36 @@
         <v>44</v>
       </c>
       <c r="D225" s="120" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E225" s="121" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F225" s="121" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="G225" s="121" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="H225" s="122"/>
       <c r="I225" s="36" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="J225" s="123" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="K225" s="124"/>
       <c r="L225" s="124"/>
       <c r="M225" s="123"/>
       <c r="N225" s="123"/>
       <c r="O225" s="124" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="P225" s="124"/>
       <c r="Q225" s="124"/>
       <c r="R225" s="124"/>
       <c r="S225" s="124" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="T225" s="124"/>
       <c r="U225" s="124"/>
@@ -22479,7 +22487,7 @@
       <c r="W225" s="124"/>
       <c r="X225" s="124"/>
       <c r="Y225" s="123" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="Z225" s="124"/>
       <c r="AA225" s="124"/>
@@ -22515,23 +22523,23 @@
         <v>44</v>
       </c>
       <c r="D226" s="120" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E226" s="121" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="F226" s="121" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="G226" s="121" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="H226" s="122"/>
       <c r="I226" s="36" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="J226" s="123" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K226" s="124"/>
       <c r="L226" s="124"/>
@@ -22544,7 +22552,7 @@
       <c r="Q226" s="124"/>
       <c r="R226" s="124"/>
       <c r="S226" s="124" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="T226" s="124"/>
       <c r="U226" s="124"/>
@@ -22552,7 +22560,7 @@
       <c r="W226" s="124"/>
       <c r="X226" s="124"/>
       <c r="Y226" s="123" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="Z226" s="124"/>
       <c r="AA226" s="124"/>
@@ -22588,36 +22596,36 @@
         <v>44</v>
       </c>
       <c r="D227" s="120" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E227" s="121" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F227" s="121" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="G227" s="121" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="H227" s="122"/>
       <c r="I227" s="36" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="J227" s="123" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K227" s="124"/>
       <c r="L227" s="124"/>
       <c r="M227" s="123"/>
       <c r="N227" s="123"/>
       <c r="O227" s="124" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="P227" s="124"/>
       <c r="Q227" s="124"/>
       <c r="R227" s="124"/>
       <c r="S227" s="124" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="T227" s="124"/>
       <c r="U227" s="124"/>
@@ -22625,7 +22633,7 @@
       <c r="W227" s="124"/>
       <c r="X227" s="124"/>
       <c r="Y227" s="123" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="Z227" s="124"/>
       <c r="AA227" s="124"/>
@@ -22661,38 +22669,38 @@
         <v>44</v>
       </c>
       <c r="D228" s="120" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E228" s="121" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F228" s="121" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="G228" s="121" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="H228" s="122" t="s">
         <v>382</v>
       </c>
       <c r="I228" s="36" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="J228" s="123" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K228" s="124"/>
       <c r="L228" s="124"/>
       <c r="M228" s="123"/>
       <c r="N228" s="123"/>
       <c r="O228" s="123" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="P228" s="124"/>
       <c r="Q228" s="124"/>
       <c r="R228" s="124"/>
       <c r="S228" s="124" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="T228" s="124"/>
       <c r="U228" s="124"/>
@@ -22700,7 +22708,7 @@
       <c r="W228" s="124"/>
       <c r="X228" s="124"/>
       <c r="Y228" s="123" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="Z228" s="124"/>
       <c r="AA228" s="124"/>
@@ -22738,38 +22746,38 @@
         <v>44</v>
       </c>
       <c r="D229" s="120" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E229" s="121" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F229" s="121" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="G229" s="121" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="H229" s="122" t="s">
         <v>409</v>
       </c>
       <c r="I229" s="36" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="J229" s="123" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K229" s="124"/>
       <c r="L229" s="124"/>
       <c r="M229" s="123"/>
       <c r="N229" s="123"/>
       <c r="O229" s="123" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="P229" s="124"/>
       <c r="Q229" s="124"/>
       <c r="R229" s="124"/>
       <c r="S229" s="124" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="T229" s="124"/>
       <c r="U229" s="124"/>
@@ -22777,7 +22785,7 @@
       <c r="W229" s="124"/>
       <c r="X229" s="124"/>
       <c r="Y229" s="123" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="Z229" s="124"/>
       <c r="AA229" s="124"/>
@@ -22815,38 +22823,38 @@
         <v>44</v>
       </c>
       <c r="D230" s="120" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E230" s="121" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F230" s="121" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="G230" s="121" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="H230" s="122" t="s">
         <v>440</v>
       </c>
       <c r="I230" s="36" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="J230" s="123" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K230" s="124"/>
       <c r="L230" s="124"/>
       <c r="M230" s="123"/>
       <c r="N230" s="123"/>
       <c r="O230" s="123" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="P230" s="124"/>
       <c r="Q230" s="124"/>
       <c r="R230" s="124"/>
       <c r="S230" s="124" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="T230" s="124"/>
       <c r="U230" s="124"/>
@@ -22854,7 +22862,7 @@
       <c r="W230" s="124"/>
       <c r="X230" s="124"/>
       <c r="Y230" s="123" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="Z230" s="124"/>
       <c r="AA230" s="124"/>
@@ -22892,38 +22900,38 @@
         <v>44</v>
       </c>
       <c r="D231" s="120" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E231" s="121" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F231" s="121" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="G231" s="121" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="H231" s="122" t="s">
         <v>458</v>
       </c>
       <c r="I231" s="36" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="J231" s="123" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K231" s="124"/>
       <c r="L231" s="124"/>
       <c r="M231" s="123"/>
       <c r="N231" s="123"/>
       <c r="O231" s="123" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="P231" s="124"/>
       <c r="Q231" s="124"/>
       <c r="R231" s="124"/>
       <c r="S231" s="124" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="T231" s="124"/>
       <c r="U231" s="124"/>
@@ -22931,7 +22939,7 @@
       <c r="W231" s="124"/>
       <c r="X231" s="124"/>
       <c r="Y231" s="131" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="Z231" s="124"/>
       <c r="AA231" s="124"/>
@@ -22969,38 +22977,38 @@
         <v>44</v>
       </c>
       <c r="D232" s="120" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E232" s="121" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F232" s="121" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="G232" s="121" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="H232" s="122" t="s">
         <v>476</v>
       </c>
       <c r="I232" s="36" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="J232" s="123" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K232" s="124"/>
       <c r="L232" s="124"/>
       <c r="M232" s="123"/>
       <c r="N232" s="123"/>
       <c r="O232" s="123" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="P232" s="124"/>
       <c r="Q232" s="124"/>
       <c r="R232" s="124"/>
       <c r="S232" s="124" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="T232" s="124"/>
       <c r="U232" s="124"/>
@@ -23008,7 +23016,7 @@
       <c r="W232" s="124"/>
       <c r="X232" s="124"/>
       <c r="Y232" s="123" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="Z232" s="124"/>
       <c r="AA232" s="124"/>
@@ -23046,38 +23054,38 @@
         <v>44</v>
       </c>
       <c r="D233" s="120" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E233" s="121" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F233" s="121" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="G233" s="121" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="H233" s="122" t="s">
         <v>488</v>
       </c>
       <c r="I233" s="36" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="J233" s="123" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K233" s="124"/>
       <c r="L233" s="124"/>
       <c r="M233" s="123"/>
       <c r="N233" s="123"/>
       <c r="O233" s="123" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="P233" s="124"/>
       <c r="Q233" s="124"/>
       <c r="R233" s="124"/>
       <c r="S233" s="124" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="T233" s="124"/>
       <c r="U233" s="124"/>
@@ -23085,7 +23093,7 @@
       <c r="W233" s="124"/>
       <c r="X233" s="124"/>
       <c r="Y233" s="123" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="Z233" s="124"/>
       <c r="AA233" s="124"/>
@@ -23123,38 +23131,38 @@
         <v>44</v>
       </c>
       <c r="D234" s="120" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E234" s="121" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F234" s="121" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="G234" s="121" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="H234" s="122" t="s">
         <v>499</v>
       </c>
       <c r="I234" s="36" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="J234" s="123" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="K234" s="124"/>
       <c r="L234" s="124"/>
       <c r="M234" s="123"/>
       <c r="N234" s="123"/>
       <c r="O234" s="123" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="P234" s="124"/>
       <c r="Q234" s="124"/>
       <c r="R234" s="124"/>
       <c r="S234" s="124" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="T234" s="124"/>
       <c r="U234" s="124"/>
@@ -23162,7 +23170,7 @@
       <c r="W234" s="124"/>
       <c r="X234" s="124"/>
       <c r="Y234" s="123" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="Z234" s="124"/>
       <c r="AA234" s="124"/>
@@ -23276,10 +23284,10 @@
         <v>13</v>
       </c>
       <c r="G1" s="134" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="H1" s="134" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="I1" s="134" t="s">
         <v>34</v>
@@ -23288,7 +23296,7 @@
         <v>31</v>
       </c>
       <c r="K1" s="134" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="L1" s="134" t="s">
         <v>35</v>
@@ -23299,7 +23307,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="135" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CCRU - KPI template update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/Supermarket PoS 2018.xlsx
+++ b/Projects/CCRU/Data/Supermarket PoS 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Supermarket" sheetId="1" state="visible" r:id="rId2"/>
@@ -44,6 +44,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Supermarket!$A$1:$AR$234</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Supermarket!$A$1:$AR$234</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Supermarket!$A$1:$AR$234</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Supermarket!$A$1:$AR$234</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -3218,23 +3219,23 @@
   <dimension ref="A1:AQ65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="N242" activeCellId="0" sqref="N242"/>
+      <selection pane="bottomLeft" activeCell="K177" activeCellId="0" sqref="K177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="5" min="1" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="13" min="11" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.7085020242915"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="34" min="16" style="0" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.3522267206478"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="36" style="0" width="9.31983805668016"/>
   </cols>
   <sheetData>
@@ -18458,7 +18459,7 @@
       </c>
       <c r="J177" s="59"/>
       <c r="K177" s="59" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L177" s="59"/>
       <c r="M177" s="59"/>

</xml_diff>